<commit_message>
finally excel sheet too
</commit_message>
<xml_diff>
--- a/SCOCS RESULT.xlsx
+++ b/SCOCS RESULT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M. Kashif Javed\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Hosted Website Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,9 +53,6 @@
     <t>MR KASHIF</t>
   </si>
   <si>
-    <t>MS UMAIR</t>
-  </si>
-  <si>
     <t>MR SAEED</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>MR UMAIR</t>
   </si>
 </sst>
 </file>
@@ -342,33 +342,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -389,6 +362,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -687,7 +687,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -700,12 +700,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
+      <c r="A1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="13"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -720,220 +720,220 @@
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="33" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="D4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="13" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2.3359999999999999</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1.9410000000000001</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2.1190000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2.3119999999999998</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2.6230000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6">
+        <v>3.1930000000000001</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2.1760000000000002</v>
+      </c>
+      <c r="E7" s="6">
+        <v>2.6349999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="6">
+        <v>2.9790000000000001</v>
+      </c>
+      <c r="D8" s="6">
+        <v>2.8180000000000001</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6">
+        <v>2.6709999999999998</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="E9" s="6">
+        <v>2.194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3.0430000000000001</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2.1349999999999998</v>
+      </c>
+      <c r="E10" s="6">
+        <v>2.5449999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6">
+        <v>2.4140000000000001</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2.9</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2.681</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6">
+        <v>3.4140000000000001</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2.9940000000000002</v>
+      </c>
+      <c r="E12" s="6">
+        <v>3.1840000000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="6">
+        <v>3.5430000000000001</v>
+      </c>
+      <c r="D13" s="6">
+        <v>3.5590000000000002</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3.4420000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6">
+        <v>2.9590000000000001</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3.145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="15">
-        <v>2.3359999999999999</v>
-      </c>
-      <c r="D5" s="15">
-        <v>1.9410000000000001</v>
-      </c>
-      <c r="E5" s="15">
-        <v>2.1190000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="16">
-        <v>3</v>
-      </c>
-      <c r="D6" s="15">
-        <v>2.3119999999999998</v>
-      </c>
-      <c r="E6" s="15">
-        <v>2.6230000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="15">
-        <v>3.1930000000000001</v>
-      </c>
-      <c r="D7" s="15">
-        <v>2.1760000000000002</v>
-      </c>
-      <c r="E7" s="15">
-        <v>2.6349999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="15">
-        <v>2.9790000000000001</v>
-      </c>
-      <c r="D8" s="15">
-        <v>2.8180000000000001</v>
-      </c>
-      <c r="E8" s="16">
-        <v>2.89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="15">
-        <v>2.6709999999999998</v>
-      </c>
-      <c r="D9" s="16">
-        <v>1.8</v>
-      </c>
-      <c r="E9" s="15">
-        <v>2.194</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="15">
-        <v>3.0430000000000001</v>
-      </c>
-      <c r="D10" s="15">
-        <v>2.1349999999999998</v>
-      </c>
-      <c r="E10" s="15">
-        <v>2.5449999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="15">
-        <v>2.4140000000000001</v>
-      </c>
-      <c r="D11" s="16">
-        <v>2.9</v>
-      </c>
-      <c r="E11" s="15">
-        <v>2.681</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="15">
-        <v>3.4140000000000001</v>
-      </c>
-      <c r="D12" s="15">
-        <v>2.9940000000000002</v>
-      </c>
-      <c r="E12" s="15">
-        <v>3.1840000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="15">
-        <v>3.5430000000000001</v>
-      </c>
-      <c r="D13" s="15">
-        <v>3.5590000000000002</v>
-      </c>
-      <c r="E13" s="15">
-        <v>3.4420000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
+      <c r="C15" s="6">
+        <v>3.4790000000000001</v>
+      </c>
+      <c r="D15" s="6">
+        <v>2.871</v>
+      </c>
+      <c r="E15" s="6">
+        <v>3.145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="15">
-        <v>2.9590000000000001</v>
-      </c>
-      <c r="E14" s="15">
-        <v>3.145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="15">
-        <v>3.4790000000000001</v>
-      </c>
-      <c r="D15" s="15">
-        <v>2.871</v>
-      </c>
-      <c r="E15" s="15">
-        <v>3.145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
+      <c r="C16" s="6">
+        <v>3.5790000000000002</v>
+      </c>
+      <c r="D16" s="6">
+        <v>3.0409999999999999</v>
+      </c>
+      <c r="E16" s="6">
+        <v>3.2839999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="15">
-        <v>3.5790000000000002</v>
-      </c>
-      <c r="D16" s="15">
-        <v>3.0409999999999999</v>
-      </c>
-      <c r="E16" s="15">
-        <v>3.2839999999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="15">
+      <c r="C17" s="6">
         <v>2.964</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="6">
         <v>3.3239999999999998</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="6">
         <v>3.161</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
+      <c r="A19" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="19"/>
     </row>
     <row r="20" spans="1:7" ht="17.25" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>

</xml_diff>

<commit_message>
replacing of s with r again
</commit_message>
<xml_diff>
--- a/SCOCS RESULT.xlsx
+++ b/SCOCS RESULT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M. Kashif Javed\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M. Kashif Javed\Documents\itdot.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,9 +53,6 @@
     <t>MR KASHIF</t>
   </si>
   <si>
-    <t>MS UMAIR</t>
-  </si>
-  <si>
     <t>MR SAEED</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>MR UMAIR</t>
   </si>
 </sst>
 </file>
@@ -378,19 +378,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -695,7 +695,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="E2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -714,7 +714,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -731,7 +731,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I4" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
@@ -746,12 +746,12 @@
       <c r="N5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="I6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
+      <c r="I6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="16"/>
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -759,13 +759,13 @@
         <v>0</v>
       </c>
       <c r="J7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="L7" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -882,7 +882,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I16" s="5" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="J16" s="6">
         <v>3.5430000000000001</v>
@@ -896,10 +896,10 @@
     </row>
     <row r="17" spans="7:14" x14ac:dyDescent="0.3">
       <c r="I17" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K17" s="6">
         <v>2.9590000000000001</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="18" spans="7:14" x14ac:dyDescent="0.3">
       <c r="I18" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J18" s="6">
         <v>3.4790000000000001</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="19" spans="7:14" x14ac:dyDescent="0.3">
       <c r="I19" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J19" s="6">
         <v>3.5790000000000002</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="20" spans="7:14" x14ac:dyDescent="0.3">
       <c r="I20" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J20" s="6">
         <v>2.964</v>
@@ -950,20 +950,20 @@
         <v>3.161</v>
       </c>
       <c r="N20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="7:14" x14ac:dyDescent="0.3">
-      <c r="G22" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="15"/>
+      <c r="G22" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>